<commit_message>
This explains when XLOOKUP can return a dynamic array
</commit_message>
<xml_diff>
--- a/XLOOKUP_An_Array.xlsx
+++ b/XLOOKUP_An_Array.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey\Desktop\Toss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B9A2D106-B210-41AC-B837-0C4969ACE60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2E9792-C456-4793-82A0-5CFBE2D69FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35820" yWindow="60" windowWidth="21600" windowHeight="12675" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-25050" yWindow="0" windowWidth="21600" windowHeight="15480" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="XLOOKUP" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Item</t>
   </si>
@@ -86,13 +86,16 @@
   </si>
   <si>
     <t>Lemon</t>
+  </si>
+  <si>
+    <t>This will return an entire array if it IS an array. This makes sense.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -182,6 +185,13 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -282,7 +292,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -290,6 +300,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comment" xfId="8" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -608,10 +619,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -773,6 +784,11 @@
         <v>Craig</v>
       </c>
     </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>